<commit_message>
updated filepaths in config
</commit_message>
<xml_diff>
--- a/templates/jiraissues.xlsx
+++ b/templates/jiraissues.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K108"/>
+  <dimension ref="A1:K105"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -493,7 +493,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>SKK-382</t>
+          <t>SKK-388</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -542,7 +542,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>SKK-381</t>
+          <t>SKK-387</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -591,7 +591,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>SKK-380</t>
+          <t>SKK-386</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -640,7 +640,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>SKK-379</t>
+          <t>SKK-385</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -689,7 +689,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>SKK-378</t>
+          <t>SKK-384</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -738,7 +738,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>SKK-377</t>
+          <t>SKK-383</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -783,171 +783,28 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>SKK-376</t>
+          <t>SKK-350</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Create StakeholderMapping</t>
+          <t>WILH Annotation Problem - Blocks LLM Transition</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Sub-task</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Project Set up</t>
-        </is>
-      </c>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr">
         <is>
           <t>To Do</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>2024-03-01</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>2024-03-06</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>stephan.kuche</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>SKK-375</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Project Set up</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Task</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Project Management</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>To Do</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>2024-03-01</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>2024-03-06</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>stephan.kuche</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>SKK-374</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Project Management</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Epic</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>To Do</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>2024-03-01</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>2024-03-06</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>stephan.kuche</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>SKK-350</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>WILH Annotation Problem - Blocks LLM Transition</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Task</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>To Do</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr">
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr">
         <is>
           <t xml:space="preserve">*Current Problem:* 
 We do not have reliable Ground Truth Data that can be used for annotation in Training projects.
@@ -967,6 +824,130 @@
 </t>
         </is>
       </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>stephan.kuche</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>SKK-349</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Assessement / Technical WS Deck</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+* error codes validations wie nach xSuite übertragen </t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>stephan.kuche</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>SKK-348</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Update infos for WIL - how to add users, how to change request.</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Sub-task</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>OPen items</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>stephan.kuche</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>SKK-347</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>derivation to update bank account informaiton from iban</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Sub-task</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>OPen items</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>To Do</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr">
         <is>
           <t>stephan.kuche</t>
@@ -982,39 +963,46 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>SKK-349</t>
+          <t>SKK-264</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Assessement / Technical WS Deck</t>
+          <t>fams tickedts erstellen</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Task</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr"/>
+          <t>Sub-task</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>OPen items</t>
+        </is>
+      </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Done</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-* error codes validations wie nach xSuite übertragen </t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>stephan.kuche</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr"/>
+          <t>To Do</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>2023-10-17</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>2023-10-17</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Tesst</t>
+        </is>
+      </c>
       <c r="K12" t="inlineStr">
         <is>
           <t>[]</t>
@@ -1024,12 +1012,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>SKK-348</t>
+          <t>SKK-263</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Update infos for WIL - how to add users, how to change request.</t>
+          <t xml:space="preserve">Ktm  Upload kickoff Sharepoint </t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -1047,15 +1035,23 @@
           <t>Done</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2023-10-17</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>2023-10-17</t>
+        </is>
+      </c>
       <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>stephan.kuche</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>asda</t>
+        </is>
+      </c>
       <c r="K13" t="inlineStr">
         <is>
           <t>[]</t>
@@ -1065,12 +1061,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>SKK-347</t>
+          <t>SKK-262</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>derivation to update bank account informaiton from iban</t>
+          <t>model renaming in the documentation</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1085,17 +1081,13 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>To Do</t>
+          <t>Done</t>
         </is>
       </c>
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>stephan.kuche</t>
-        </is>
-      </c>
+      <c r="I14" t="inlineStr"/>
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr">
         <is>
@@ -1106,12 +1098,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>SKK-264</t>
+          <t>SKK-261</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>fams tickedts erstellen</t>
+          <t>backend topic - training projects</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1129,23 +1121,15 @@
           <t>To Do</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>2023-10-17</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>2023-10-17</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">[https://hypatos.atlassian.net/browse/BACKEND-581|https://hypatos.atlassian.net/browse/BACKEND-581|smart-link] </t>
+        </is>
+      </c>
       <c r="I15" t="inlineStr"/>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>Tesst</t>
-        </is>
-      </c>
+      <c r="J15" t="inlineStr"/>
       <c r="K15" t="inlineStr">
         <is>
           <t>[]</t>
@@ -1155,12 +1139,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>SKK-263</t>
+          <t>SKK-260</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t xml:space="preserve">Ktm  Upload kickoff Sharepoint </t>
+          <t>Clarify Tax Table</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1175,26 +1159,14 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Done</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>2023-10-17</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>2023-10-17</t>
-        </is>
-      </c>
+          <t>To Do</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr"/>
       <c r="I16" t="inlineStr"/>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>asda</t>
-        </is>
-      </c>
+      <c r="J16" t="inlineStr"/>
       <c r="K16" t="inlineStr">
         <is>
           <t>[]</t>
@@ -1204,12 +1176,12 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>SKK-262</t>
+          <t>SKK-259</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>model renaming in the documentation</t>
+          <t>Regex for Company Names</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1241,12 +1213,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>SKK-261</t>
+          <t>SKK-258</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>backend topic - training projects</t>
+          <t>Save validation schema totals tax  totals Gross</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1261,127 +1233,12 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>To Do</t>
+          <t>Done</t>
         </is>
       </c>
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr"/>
       <c r="H18" t="inlineStr">
-        <is>
-          <t xml:space="preserve">[https://hypatos.atlassian.net/browse/BACKEND-581|https://hypatos.atlassian.net/browse/BACKEND-581|smart-link] </t>
-        </is>
-      </c>
-      <c r="I18" t="inlineStr"/>
-      <c r="J18" t="inlineStr"/>
-      <c r="K18" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>SKK-260</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Clarify Tax Table</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Sub-task</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>OPen items</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>To Do</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr"/>
-      <c r="G19" t="inlineStr"/>
-      <c r="H19" t="inlineStr"/>
-      <c r="I19" t="inlineStr"/>
-      <c r="J19" t="inlineStr"/>
-      <c r="K19" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>SKK-259</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Regex for Company Names</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Sub-task</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>OPen items</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>Done</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr"/>
-      <c r="G20" t="inlineStr"/>
-      <c r="H20" t="inlineStr"/>
-      <c r="I20" t="inlineStr"/>
-      <c r="J20" t="inlineStr"/>
-      <c r="K20" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>SKK-258</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Save validation schema totals tax  totals Gross</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>Sub-task</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>OPen items</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>Done</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr"/>
-      <c r="G21" t="inlineStr"/>
-      <c r="H21" t="inlineStr">
         <is>
           <t>{noformat}{
                     "internalName": "gross",
@@ -1421,6 +1278,113 @@
                 },{noformat}</t>
         </is>
       </c>
+      <c r="I18" t="inlineStr"/>
+      <c r="J18" t="inlineStr"/>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>SKK-257</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ticket supplier master data wilh </t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Sub-task</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>OPen items</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>no problem detectd</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr"/>
+      <c r="J19" t="inlineStr"/>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>SKK-256</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>OPen items</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>To Do</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr"/>
+      <c r="G20" t="inlineStr"/>
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="inlineStr"/>
+      <c r="J20" t="inlineStr"/>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>SKK-87</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>[WILH] implement totals net - total gross validation</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>In Progress</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr"/>
+      <c r="G21" t="inlineStr"/>
+      <c r="H21" t="inlineStr"/>
       <c r="I21" t="inlineStr"/>
       <c r="J21" t="inlineStr"/>
       <c r="K21" t="inlineStr">
@@ -1432,12 +1396,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>SKK-257</t>
+          <t>SKK-86</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t xml:space="preserve">Ticket supplier master data wilh </t>
+          <t>Invite external users to JWM</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1447,7 +1411,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>OPen items</t>
+          <t>[FUNKE]</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1457,11 +1421,7 @@
       </c>
       <c r="F22" t="inlineStr"/>
       <c r="G22" t="inlineStr"/>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>no problem detectd</t>
-        </is>
-      </c>
+      <c r="H22" t="inlineStr"/>
       <c r="I22" t="inlineStr"/>
       <c r="J22" t="inlineStr"/>
       <c r="K22" t="inlineStr">
@@ -1473,23 +1433,27 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>SKK-256</t>
+          <t>SKK-85</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>OPen items</t>
+          <t>Create Jira (JWM) Project</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Task</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr"/>
+          <t>Sub-task</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>[FUNKE]</t>
+        </is>
+      </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>To Do</t>
+          <t>Done</t>
         </is>
       </c>
       <c r="F23" t="inlineStr"/>
@@ -1506,23 +1470,27 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>SKK-87</t>
+          <t>SKK-84</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>[WILH] implement totals net - total gross validation</t>
+          <t>Create JourFixe PMO &amp; Steerco Meeting Series</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Task</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr"/>
+          <t>Sub-task</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>[FUNKE]</t>
+        </is>
+      </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>In Progress</t>
+          <t>Done</t>
         </is>
       </c>
       <c r="F24" t="inlineStr"/>
@@ -1539,12 +1507,12 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>SKK-86</t>
+          <t>SKK-83</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Invite external users to JWM</t>
+          <t>Schedule Workshops (AWS, FWS, TWS)</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1576,12 +1544,12 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>SKK-85</t>
+          <t>SKK-82</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Create Jira (JWM) Project</t>
+          <t>Hy Academy Access</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1613,12 +1581,12 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>SKK-84</t>
+          <t>SKK-81</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Create JourFixe PMO &amp; Steerco Meeting Series</t>
+          <t>Stakeholder mappijng</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1650,12 +1618,12 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>SKK-83</t>
+          <t>SKK-80</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Schedule Workshops (AWS, FWS, TWS)</t>
+          <t xml:space="preserve">Sharpoint Page </t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1687,12 +1655,12 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>SKK-82</t>
+          <t>SKK-79</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Hy Academy Access</t>
+          <t>Absence Planner</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1711,7 +1679,11 @@
         </is>
       </c>
       <c r="F29" t="inlineStr"/>
-      <c r="G29" t="inlineStr"/>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>2023-12-22</t>
+        </is>
+      </c>
       <c r="H29" t="inlineStr"/>
       <c r="I29" t="inlineStr"/>
       <c r="J29" t="inlineStr"/>
@@ -1724,12 +1696,12 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>SKK-81</t>
+          <t>SKK-78</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Stakeholder mappijng</t>
+          <t>Update Slidedeck Kickoff</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1761,12 +1733,12 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>SKK-80</t>
+          <t>SKK-77</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t xml:space="preserve">Sharpoint Page </t>
+          <t>Welche Buchungskreise und top vendoren sind relevant</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1798,12 +1770,12 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>SKK-79</t>
+          <t>SKK-76</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Absence Planner</t>
+          <t>Create RAID log</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1822,11 +1794,7 @@
         </is>
       </c>
       <c r="F32" t="inlineStr"/>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>2023-12-22</t>
-        </is>
-      </c>
+      <c r="G32" t="inlineStr"/>
       <c r="H32" t="inlineStr"/>
       <c r="I32" t="inlineStr"/>
       <c r="J32" t="inlineStr"/>
@@ -1839,12 +1807,12 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>SKK-78</t>
+          <t>SKK-75</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Update Slidedeck Kickoff</t>
+          <t>teams &amp; sharepoint und externe user zulassen</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1876,12 +1844,12 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>SKK-77</t>
+          <t>SKK-74</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Welche Buchungskreise und top vendoren sind relevant</t>
+          <t>credentials versenden</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1913,12 +1881,12 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>SKK-76</t>
+          <t>SKK-73</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Create RAID log</t>
+          <t>credentials erstellen</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1950,12 +1918,12 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>SKK-75</t>
+          <t>SKK-72</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>teams &amp; sharepoint und externe user zulassen</t>
+          <t>Send SAP Addon (Install + SP1)</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1987,12 +1955,12 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>SKK-74</t>
+          <t>SKK-71</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>credentials versenden</t>
+          <t>doku SAP raussenden</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -2024,12 +1992,12 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>SKK-73</t>
+          <t>SKK-70</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>credentials erstellen</t>
+          <t>sap certificates - name von SAP basis guy an dawid</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -2061,33 +2029,33 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>SKK-72</t>
+          <t>SKK-69</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Send SAP Addon (Install + SP1)</t>
+          <t>[FUNKE]</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Sub-task</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>[FUNKE]</t>
-        </is>
-      </c>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr"/>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Done</t>
+          <t>To Do</t>
         </is>
       </c>
       <c r="F39" t="inlineStr"/>
       <c r="G39" t="inlineStr"/>
       <c r="H39" t="inlineStr"/>
-      <c r="I39" t="inlineStr"/>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>stephan.kuche</t>
+        </is>
+      </c>
       <c r="J39" t="inlineStr"/>
       <c r="K39" t="inlineStr">
         <is>
@@ -2098,27 +2066,23 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>SKK-71</t>
+          <t>SKK-68</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>doku SAP raussenden</t>
+          <t>[WILH] Update PO Number rule - currently captures to many chars</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Sub-task</t>
-        </is>
-      </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>[FUNKE]</t>
-        </is>
-      </c>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr"/>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Done</t>
+          <t>To Do</t>
         </is>
       </c>
       <c r="F40" t="inlineStr"/>
@@ -2135,135 +2099,28 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>SKK-70</t>
+          <t>SKK-67</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>sap certificates - name von SAP basis guy an dawid</t>
+          <t>[OKR] Steps</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Sub-task</t>
-        </is>
-      </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>[FUNKE]</t>
-        </is>
-      </c>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr"/>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Done</t>
+          <t>In Progress</t>
         </is>
       </c>
       <c r="F41" t="inlineStr"/>
       <c r="G41" t="inlineStr"/>
-      <c r="H41" t="inlineStr"/>
-      <c r="I41" t="inlineStr"/>
-      <c r="J41" t="inlineStr"/>
-      <c r="K41" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>SKK-69</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>[FUNKE]</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>Task</t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr"/>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>To Do</t>
-        </is>
-      </c>
-      <c r="F42" t="inlineStr"/>
-      <c r="G42" t="inlineStr"/>
-      <c r="H42" t="inlineStr"/>
-      <c r="I42" t="inlineStr">
-        <is>
-          <t>stephan.kuche</t>
-        </is>
-      </c>
-      <c r="J42" t="inlineStr"/>
-      <c r="K42" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>SKK-68</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>[WILH] Update PO Number rule - currently captures to many chars</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>Task</t>
-        </is>
-      </c>
-      <c r="D43" t="inlineStr"/>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>To Do</t>
-        </is>
-      </c>
-      <c r="F43" t="inlineStr"/>
-      <c r="G43" t="inlineStr"/>
-      <c r="H43" t="inlineStr"/>
-      <c r="I43" t="inlineStr"/>
-      <c r="J43" t="inlineStr"/>
-      <c r="K43" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>SKK-67</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>[OKR] Steps</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>Task</t>
-        </is>
-      </c>
-      <c r="D44" t="inlineStr"/>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>In Progress</t>
-        </is>
-      </c>
-      <c r="F44" t="inlineStr"/>
-      <c r="G44" t="inlineStr"/>
-      <c r="H44" t="inlineStr">
+      <c r="H41" t="inlineStr">
         <is>
           <t xml:space="preserve">Hi Leticia 
 here are the steps that need to be performed
@@ -2280,105 +2137,105 @@
  </t>
         </is>
       </c>
-      <c r="I44" t="inlineStr"/>
-      <c r="J44" t="inlineStr"/>
-      <c r="K44" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
+      <c r="I41" t="inlineStr"/>
+      <c r="J41" t="inlineStr"/>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
         <is>
           <t>SKK-66</t>
         </is>
       </c>
-      <c r="B45" t="inlineStr">
+      <c r="B42" t="inlineStr">
         <is>
           <t>[WIL] Insert Dummy Supplier</t>
         </is>
       </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>Task</t>
-        </is>
-      </c>
-      <c r="D45" t="inlineStr"/>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>Done</t>
-        </is>
-      </c>
-      <c r="F45" t="inlineStr"/>
-      <c r="G45" t="inlineStr"/>
-      <c r="H45" t="inlineStr"/>
-      <c r="I45" t="inlineStr"/>
-      <c r="J45" t="inlineStr"/>
-      <c r="K45" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr"/>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr"/>
+      <c r="G42" t="inlineStr"/>
+      <c r="H42" t="inlineStr"/>
+      <c r="I42" t="inlineStr"/>
+      <c r="J42" t="inlineStr"/>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
         <is>
           <t>SKK-64</t>
         </is>
       </c>
-      <c r="B46" t="inlineStr">
+      <c r="B43" t="inlineStr">
         <is>
           <t>[WIL] delete company validation JP</t>
         </is>
       </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>Task</t>
-        </is>
-      </c>
-      <c r="D46" t="inlineStr"/>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>Done</t>
-        </is>
-      </c>
-      <c r="F46" t="inlineStr"/>
-      <c r="G46" t="inlineStr"/>
-      <c r="H46" t="inlineStr"/>
-      <c r="I46" t="inlineStr"/>
-      <c r="J46" t="inlineStr"/>
-      <c r="K46" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr"/>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr"/>
+      <c r="G43" t="inlineStr"/>
+      <c r="H43" t="inlineStr"/>
+      <c r="I43" t="inlineStr"/>
+      <c r="J43" t="inlineStr"/>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
         <is>
           <t>SKK-63</t>
         </is>
       </c>
-      <c r="B47" t="inlineStr">
+      <c r="B44" t="inlineStr">
         <is>
           <t>[WIL] JP Model enhancement</t>
         </is>
       </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>Task</t>
-        </is>
-      </c>
-      <c r="D47" t="inlineStr"/>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>Done</t>
-        </is>
-      </c>
-      <c r="F47" t="inlineStr"/>
-      <c r="G47" t="inlineStr"/>
-      <c r="H47" t="inlineStr">
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr"/>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr"/>
+      <c r="G44" t="inlineStr"/>
+      <c r="H44" t="inlineStr">
         <is>
           <t>* annotate a second version of document
 * maybe use local finance or posting data
@@ -2386,39 +2243,39 @@
 * get back to He</t>
         </is>
       </c>
-      <c r="I47" t="inlineStr"/>
-      <c r="J47" t="inlineStr"/>
-      <c r="K47" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
+      <c r="I44" t="inlineStr"/>
+      <c r="J44" t="inlineStr"/>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
         <is>
           <t>SKK-62</t>
         </is>
       </c>
-      <c r="B48" t="inlineStr">
+      <c r="B45" t="inlineStr">
         <is>
           <t xml:space="preserve">[WIL] Cutover Plan </t>
         </is>
       </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>Task</t>
-        </is>
-      </c>
-      <c r="D48" t="inlineStr"/>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>Done</t>
-        </is>
-      </c>
-      <c r="F48" t="inlineStr"/>
-      <c r="G48" t="inlineStr"/>
-      <c r="H48" t="inlineStr">
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr"/>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr"/>
+      <c r="G45" t="inlineStr"/>
+      <c r="H45" t="inlineStr">
         <is>
           <t xml:space="preserve">
 * feature flags ( must correct all errrors )
@@ -2435,72 +2292,72 @@
 * create dashboards</t>
         </is>
       </c>
-      <c r="I48" t="inlineStr"/>
-      <c r="J48" t="inlineStr"/>
-      <c r="K48" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
+      <c r="I45" t="inlineStr"/>
+      <c r="J45" t="inlineStr"/>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
         <is>
           <t>SKK-61</t>
         </is>
       </c>
-      <c r="B49" t="inlineStr">
+      <c r="B46" t="inlineStr">
         <is>
           <t>[WIL] Deploy JP model to test env</t>
         </is>
       </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>Task</t>
-        </is>
-      </c>
-      <c r="D49" t="inlineStr"/>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>Done</t>
-        </is>
-      </c>
-      <c r="F49" t="inlineStr"/>
-      <c r="G49" t="inlineStr"/>
-      <c r="H49" t="inlineStr"/>
-      <c r="I49" t="inlineStr"/>
-      <c r="J49" t="inlineStr"/>
-      <c r="K49" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr"/>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr"/>
+      <c r="G46" t="inlineStr"/>
+      <c r="H46" t="inlineStr"/>
+      <c r="I46" t="inlineStr"/>
+      <c r="J46" t="inlineStr"/>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
         <is>
           <t>SKK-60</t>
         </is>
       </c>
-      <c r="B50" t="inlineStr">
+      <c r="B47" t="inlineStr">
         <is>
           <t>[WIL] USER training I &amp; II</t>
         </is>
       </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>Task</t>
-        </is>
-      </c>
-      <c r="D50" t="inlineStr"/>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t>Done</t>
-        </is>
-      </c>
-      <c r="F50" t="inlineStr"/>
-      <c r="G50" t="inlineStr"/>
-      <c r="H50" t="inlineStr">
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr"/>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr"/>
+      <c r="G47" t="inlineStr"/>
+      <c r="H47" t="inlineStr">
         <is>
           <t>* Access and Login 
 * User Roles and different permissions
@@ -2531,72 +2388,72 @@
 * what to do / what not to do</t>
         </is>
       </c>
-      <c r="I50" t="inlineStr"/>
-      <c r="J50" t="inlineStr"/>
-      <c r="K50" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
+      <c r="I47" t="inlineStr"/>
+      <c r="J47" t="inlineStr"/>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
         <is>
           <t>SKK-59</t>
         </is>
       </c>
-      <c r="B51" t="inlineStr">
+      <c r="B48" t="inlineStr">
         <is>
           <t>[WIL] Reduce Schema in Gateway</t>
         </is>
       </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>Task</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr"/>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>Done</t>
-        </is>
-      </c>
-      <c r="F51" t="inlineStr"/>
-      <c r="G51" t="inlineStr"/>
-      <c r="H51" t="inlineStr"/>
-      <c r="I51" t="inlineStr"/>
-      <c r="J51" t="inlineStr"/>
-      <c r="K51" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr"/>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr"/>
+      <c r="G48" t="inlineStr"/>
+      <c r="H48" t="inlineStr"/>
+      <c r="I48" t="inlineStr"/>
+      <c r="J48" t="inlineStr"/>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
         <is>
           <t>SKK-58</t>
         </is>
       </c>
-      <c r="B52" t="inlineStr">
+      <c r="B49" t="inlineStr">
         <is>
           <t>[WIL] Test Feedback</t>
         </is>
       </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>Task</t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr"/>
-      <c r="E52" t="inlineStr">
-        <is>
-          <t>Done</t>
-        </is>
-      </c>
-      <c r="F52" t="inlineStr"/>
-      <c r="G52" t="inlineStr"/>
-      <c r="H52" t="inlineStr">
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr"/>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr"/>
+      <c r="G49" t="inlineStr"/>
+      <c r="H49" t="inlineStr">
         <is>
           <t xml:space="preserve">* involve japanese team to check supplier enrichment 
 * upload all top vendors for each entity (one sample per entity )  → let japanes account check if supplier enrichment was correct
@@ -2617,72 +2474,72 @@
 ** </t>
         </is>
       </c>
-      <c r="I52" t="inlineStr"/>
-      <c r="J52" t="inlineStr"/>
-      <c r="K52" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
+      <c r="I49" t="inlineStr"/>
+      <c r="J49" t="inlineStr"/>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
         <is>
           <t>SKK-57</t>
         </is>
       </c>
-      <c r="B53" t="inlineStr">
+      <c r="B50" t="inlineStr">
         <is>
           <t>[WIL] CreditNote - minus</t>
         </is>
       </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>Task</t>
-        </is>
-      </c>
-      <c r="D53" t="inlineStr"/>
-      <c r="E53" t="inlineStr">
-        <is>
-          <t>Done</t>
-        </is>
-      </c>
-      <c r="F53" t="inlineStr"/>
-      <c r="G53" t="inlineStr"/>
-      <c r="H53" t="inlineStr"/>
-      <c r="I53" t="inlineStr"/>
-      <c r="J53" t="inlineStr"/>
-      <c r="K53" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr"/>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr"/>
+      <c r="G50" t="inlineStr"/>
+      <c r="H50" t="inlineStr"/>
+      <c r="I50" t="inlineStr"/>
+      <c r="J50" t="inlineStr"/>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
         <is>
           <t>SKK-55</t>
         </is>
       </c>
-      <c r="B54" t="inlineStr">
+      <c r="B51" t="inlineStr">
         <is>
           <t>Contact ThinkCell - support@think-cell.com - links to ranges</t>
         </is>
       </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>Task</t>
-        </is>
-      </c>
-      <c r="D54" t="inlineStr"/>
-      <c r="E54" t="inlineStr">
-        <is>
-          <t>Done</t>
-        </is>
-      </c>
-      <c r="F54" t="inlineStr"/>
-      <c r="G54" t="inlineStr"/>
-      <c r="H54" t="inlineStr">
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr"/>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr"/>
+      <c r="G51" t="inlineStr"/>
+      <c r="H51" t="inlineStr">
         <is>
           <t xml:space="preserve">Dear think cell team,
 I am trying to achieve the following process automation but I am not sure whether this is possible. 
@@ -2696,47 +2553,47 @@
 </t>
         </is>
       </c>
-      <c r="I54" t="inlineStr"/>
-      <c r="J54" t="inlineStr"/>
-      <c r="K54" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
+      <c r="I51" t="inlineStr"/>
+      <c r="J51" t="inlineStr"/>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
         <is>
           <t>SKK-54</t>
         </is>
       </c>
-      <c r="B55" t="inlineStr">
+      <c r="B52" t="inlineStr">
         <is>
           <t>[WILH] SOlution Design Design Sign OFF3</t>
         </is>
       </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>Task</t>
-        </is>
-      </c>
-      <c r="D55" t="inlineStr"/>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>Done</t>
-        </is>
-      </c>
-      <c r="F55" t="inlineStr">
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr"/>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
         <is>
           <t>2023-11-11</t>
         </is>
       </c>
-      <c r="G55" t="inlineStr">
+      <c r="G52" t="inlineStr">
         <is>
           <t>2023-11-30</t>
         </is>
       </c>
-      <c r="H55" t="inlineStr">
+      <c r="H52" t="inlineStr">
         <is>
           <t>Question to Amadeusz - 
 # What do you actually patch when you upload a document - only externalId
@@ -2744,11 +2601,110 @@
 # are email sender etc  datapoints used  - YES</t>
         </is>
       </c>
-      <c r="I55" t="inlineStr">
+      <c r="I52" t="inlineStr">
         <is>
           <t>stephan.kuche</t>
         </is>
       </c>
+      <c r="J52" t="inlineStr"/>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>SKK-53</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>[Internal] Feedback</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr"/>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr"/>
+      <c r="G53" t="inlineStr"/>
+      <c r="H53" t="inlineStr"/>
+      <c r="I53" t="inlineStr"/>
+      <c r="J53" t="inlineStr"/>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>SKK-52</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>[WIL] Create Testing KIckoff Slidedeck</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr"/>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr"/>
+      <c r="G54" t="inlineStr"/>
+      <c r="H54" t="inlineStr"/>
+      <c r="I54" t="inlineStr"/>
+      <c r="J54" t="inlineStr"/>
+      <c r="K54" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>SKK-51</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Delete IMP JP and or link anothert index and create fingerprints again,</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr"/>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr"/>
+      <c r="G55" t="inlineStr"/>
+      <c r="H55" t="inlineStr"/>
+      <c r="I55" t="inlineStr"/>
       <c r="J55" t="inlineStr"/>
       <c r="K55" t="inlineStr">
         <is>
@@ -2759,12 +2715,12 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>SKK-53</t>
+          <t>SKK-50</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>[Internal] Feedback</t>
+          <t>[WIL] go through external Data with Amadeusz</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -2792,12 +2748,12 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>SKK-52</t>
+          <t>SKK-49</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>[WIL] Create Testing KIckoff Slidedeck</t>
+          <t>check if imp in JP is wired to PO / NON PO project</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -2811,26 +2767,34 @@
           <t>Done</t>
         </is>
       </c>
-      <c r="F57" t="inlineStr"/>
-      <c r="G57" t="inlineStr"/>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>2023-09-21</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>2023-10-07</t>
+        </is>
+      </c>
       <c r="H57" t="inlineStr"/>
       <c r="I57" t="inlineStr"/>
       <c r="J57" t="inlineStr"/>
       <c r="K57" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[{'LinkType': 'blocks', 'LinkedIssueSummary': 'Documentation of Translation Service'}]</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>SKK-51</t>
+          <t>SKK-48</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Delete IMP JP and or link anothert index and create fingerprints again,</t>
+          <t>WIL VMD - threshold if confidence too low</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -2858,12 +2822,12 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>SKK-50</t>
+          <t>SKK-47</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>[WIL] go through external Data with Amadeusz</t>
+          <t>Rouitng NON PO Invoices CoE</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -2891,12 +2855,12 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>SKK-49</t>
+          <t>SKK-46</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>check if imp in JP is wired to PO / NON PO project</t>
+          <t>WIL - discuss OC datapoints</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -2910,34 +2874,30 @@
           <t>Done</t>
         </is>
       </c>
-      <c r="F60" t="inlineStr">
-        <is>
-          <t>2023-09-21</t>
-        </is>
-      </c>
-      <c r="G60" t="inlineStr">
-        <is>
-          <t>2023-10-07</t>
-        </is>
-      </c>
-      <c r="H60" t="inlineStr"/>
+      <c r="F60" t="inlineStr"/>
+      <c r="G60" t="inlineStr"/>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>|A108|Merge Data Mapping into one file|Open|Stephan|2023-10-02|2023-10-05| |Creation of one Mapping File for Document Outbound (CML|</t>
+        </is>
+      </c>
       <c r="I60" t="inlineStr"/>
       <c r="J60" t="inlineStr"/>
       <c r="K60" t="inlineStr">
         <is>
-          <t>[{'LinkType': 'blocks', 'LinkedIssueSummary': 'Documentation of Translation Service'}]</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>SKK-48</t>
+          <t>SKK-45</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>WIL VMD - threshold if confidence too low</t>
+          <t>JP Retraining?</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -2965,12 +2925,12 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>SKK-47</t>
+          <t>SKK-44</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Rouitng NON PO Invoices CoE</t>
+          <t>VMD QA Insights -  run GH action</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -2998,12 +2958,12 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>SKK-46</t>
+          <t>SKK-43</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>WIL - discuss OC datapoints</t>
+          <t>CoE Ticket Enhance VMD Matching  ACC</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -3019,11 +2979,7 @@
       </c>
       <c r="F63" t="inlineStr"/>
       <c r="G63" t="inlineStr"/>
-      <c r="H63" t="inlineStr">
-        <is>
-          <t>|A108|Merge Data Mapping into one file|Open|Stephan|2023-10-02|2023-10-05| |Creation of one Mapping File for Document Outbound (CML|</t>
-        </is>
-      </c>
+      <c r="H63" t="inlineStr"/>
       <c r="I63" t="inlineStr"/>
       <c r="J63" t="inlineStr"/>
       <c r="K63" t="inlineStr">
@@ -3035,12 +2991,12 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>SKK-45</t>
+          <t>SKK-42</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>JP Retraining?</t>
+          <t>Discuss Routijng logic with WIL</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -3068,12 +3024,12 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>SKK-44</t>
+          <t>SKK-41</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>VMD QA Insights -  run GH action</t>
+          <t>WIL finish check routing projects</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -3101,12 +3057,12 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>SKK-43</t>
+          <t>SKK-40</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>CoE Ticket Enhance VMD Matching  ACC</t>
+          <t>WIL - Follow up with INT Ticket Denys</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -3122,7 +3078,11 @@
       </c>
       <c r="F66" t="inlineStr"/>
       <c r="G66" t="inlineStr"/>
-      <c r="H66" t="inlineStr"/>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t xml:space="preserve">[https://hypatos.atlassian.net/browse/INT-605|https://hypatos.atlassian.net/browse/INT-605|smart-link] </t>
+        </is>
+      </c>
       <c r="I66" t="inlineStr"/>
       <c r="J66" t="inlineStr"/>
       <c r="K66" t="inlineStr">
@@ -3134,12 +3094,12 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>SKK-42</t>
+          <t>SKK-39</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Discuss Routijng logic with WIL</t>
+          <t>WIL Mapping - Recipient CompanyCode</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -3155,110 +3115,7 @@
       </c>
       <c r="F67" t="inlineStr"/>
       <c r="G67" t="inlineStr"/>
-      <c r="H67" t="inlineStr"/>
-      <c r="I67" t="inlineStr"/>
-      <c r="J67" t="inlineStr"/>
-      <c r="K67" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>SKK-41</t>
-        </is>
-      </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>WIL finish check routing projects</t>
-        </is>
-      </c>
-      <c r="C68" t="inlineStr">
-        <is>
-          <t>Task</t>
-        </is>
-      </c>
-      <c r="D68" t="inlineStr"/>
-      <c r="E68" t="inlineStr">
-        <is>
-          <t>Done</t>
-        </is>
-      </c>
-      <c r="F68" t="inlineStr"/>
-      <c r="G68" t="inlineStr"/>
-      <c r="H68" t="inlineStr"/>
-      <c r="I68" t="inlineStr"/>
-      <c r="J68" t="inlineStr"/>
-      <c r="K68" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>SKK-40</t>
-        </is>
-      </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>WIL - Follow up with INT Ticket Denys</t>
-        </is>
-      </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t>Task</t>
-        </is>
-      </c>
-      <c r="D69" t="inlineStr"/>
-      <c r="E69" t="inlineStr">
-        <is>
-          <t>Done</t>
-        </is>
-      </c>
-      <c r="F69" t="inlineStr"/>
-      <c r="G69" t="inlineStr"/>
-      <c r="H69" t="inlineStr">
-        <is>
-          <t xml:space="preserve">[https://hypatos.atlassian.net/browse/INT-605|https://hypatos.atlassian.net/browse/INT-605|smart-link] </t>
-        </is>
-      </c>
-      <c r="I69" t="inlineStr"/>
-      <c r="J69" t="inlineStr"/>
-      <c r="K69" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="inlineStr">
-        <is>
-          <t>SKK-39</t>
-        </is>
-      </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>WIL Mapping - Recipient CompanyCode</t>
-        </is>
-      </c>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t>Task</t>
-        </is>
-      </c>
-      <c r="D70" t="inlineStr"/>
-      <c r="E70" t="inlineStr">
-        <is>
-          <t>Done</t>
-        </is>
-      </c>
-      <c r="F70" t="inlineStr"/>
-      <c r="G70" t="inlineStr"/>
-      <c r="H70" t="inlineStr">
+      <c r="H67" t="inlineStr">
         <is>
           <t xml:space="preserve">Frage an Fotis - 
 Was ist der letzte stand des mapping files.
@@ -3269,23 +3126,130 @@
 </t>
         </is>
       </c>
+      <c r="I67" t="inlineStr"/>
+      <c r="J67" t="inlineStr"/>
+      <c r="K67" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>SKK-38</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>[WIL] Schedule kickoff for testing</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr"/>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr"/>
+      <c r="G68" t="inlineStr"/>
+      <c r="H68" t="inlineStr"/>
+      <c r="I68" t="inlineStr"/>
+      <c r="J68" t="inlineStr"/>
+      <c r="K68" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>SKK-37</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>[WIL] testing workbook - description of terms</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr"/>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr"/>
+      <c r="G69" t="inlineStr"/>
+      <c r="H69" t="inlineStr"/>
+      <c r="I69" t="inlineStr"/>
+      <c r="J69" t="inlineStr"/>
+      <c r="K69" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>SKK-36</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Documentation of Translation Service</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr"/>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>2023-10-17</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>2023-10-31</t>
+        </is>
+      </c>
+      <c r="H70" t="inlineStr"/>
       <c r="I70" t="inlineStr"/>
       <c r="J70" t="inlineStr"/>
       <c r="K70" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[{'LinkType': 'is blocked by', 'LinkedIssueSummary': 'check if imp in JP is wired to PO / NON PO project'}]</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>SKK-38</t>
+          <t>SKK-35</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>[WIL] Schedule kickoff for testing</t>
+          <t>[WIL] add PO validation also on POLINE ITEM Level</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -3313,12 +3277,12 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>SKK-37</t>
+          <t>SKK-34</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>[WIL] testing workbook - description of terms</t>
+          <t>[WIL] Upload Documentation of Archiving to WILH Sharepoint</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -3346,12 +3310,12 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>SKK-36</t>
+          <t>SKK-33</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Documentation of Translation Service</t>
+          <t>[WIL] Share Translation Service Credentials - can be shared with customer</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -3365,34 +3329,26 @@
           <t>Done</t>
         </is>
       </c>
-      <c r="F73" t="inlineStr">
-        <is>
-          <t>2023-10-17</t>
-        </is>
-      </c>
-      <c r="G73" t="inlineStr">
-        <is>
-          <t>2023-10-31</t>
-        </is>
-      </c>
+      <c r="F73" t="inlineStr"/>
+      <c r="G73" t="inlineStr"/>
       <c r="H73" t="inlineStr"/>
       <c r="I73" t="inlineStr"/>
       <c r="J73" t="inlineStr"/>
       <c r="K73" t="inlineStr">
         <is>
-          <t>[{'LinkType': 'is blocked by', 'LinkedIssueSummary': 'check if imp in JP is wired to PO / NON PO project'}]</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>SKK-35</t>
+          <t>SKK-32</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>[WIL] add PO validation also on POLINE ITEM Level</t>
+          <t>[WIL] Translaation service to japanese projects</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -3420,12 +3376,12 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>SKK-34</t>
+          <t>SKK-31</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>[WIL] Upload Documentation of Archiving to WILH Sharepoint</t>
+          <t>[WIL] external data - derivation rule / and default values</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -3441,7 +3397,12 @@
       </c>
       <c r="F75" t="inlineStr"/>
       <c r="G75" t="inlineStr"/>
-      <c r="H75" t="inlineStr"/>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>{noformat}"externalData": {
+                "email": "gbs-finance-service-layer-sol@wilhelmsen.com"{noformat}</t>
+        </is>
+      </c>
       <c r="I75" t="inlineStr"/>
       <c r="J75" t="inlineStr"/>
       <c r="K75" t="inlineStr">
@@ -3453,20 +3414,24 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>SKK-33</t>
+          <t>SKK-30</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>[WIL] Share Translation Service Credentials - can be shared with customer</t>
+          <t>Add PO extract and Reciepient Valdiation to PO/NON invoices Project</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Task</t>
-        </is>
-      </c>
-      <c r="D76" t="inlineStr"/>
+          <t>Sub-task</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>[WIL] Studio App Setup</t>
+        </is>
+      </c>
       <c r="E76" t="inlineStr">
         <is>
           <t>Done</t>
@@ -3474,7 +3439,13 @@
       </c>
       <c r="F76" t="inlineStr"/>
       <c r="G76" t="inlineStr"/>
-      <c r="H76" t="inlineStr"/>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>other: [https://cloud.hypatos.ai/projects/po-extract-agdh8f5s|https://cloud.hypatos.ai/projects/po-extract-agdh8f5s|smart-link] 
+JP [https://cloud.hypatos.ai/projects/po-extract-jp-18lyzmdi|https://cloud.hypatos.ai/projects/po-extract-jp-18lyzmdi|smart-link] 
+valid - see companies</t>
+        </is>
+      </c>
       <c r="I76" t="inlineStr"/>
       <c r="J76" t="inlineStr"/>
       <c r="K76" t="inlineStr">
@@ -3486,12 +3457,12 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>SKK-32</t>
+          <t>SKK-29</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>[WIL] Translaation service to japanese projects</t>
+          <t>[WIL] endusers to add to studio</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -3519,12 +3490,12 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>SKK-31</t>
+          <t>SKK-28</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>[WIL] external data - derivation rule / and default values</t>
+          <t>Validation Rule - Requirement Sheet - Company Name</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -3540,12 +3511,7 @@
       </c>
       <c r="F78" t="inlineStr"/>
       <c r="G78" t="inlineStr"/>
-      <c r="H78" t="inlineStr">
-        <is>
-          <t>{noformat}"externalData": {
-                "email": "gbs-finance-service-layer-sol@wilhelmsen.com"{noformat}</t>
-        </is>
-      </c>
+      <c r="H78" t="inlineStr"/>
       <c r="I78" t="inlineStr"/>
       <c r="J78" t="inlineStr"/>
       <c r="K78" t="inlineStr">
@@ -3557,24 +3523,20 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>SKK-30</t>
+          <t>SKK-27</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Add PO extract and Reciepient Valdiation to PO/NON invoices Project</t>
+          <t>[WIL] start imp training</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Sub-task</t>
-        </is>
-      </c>
-      <c r="D79" t="inlineStr">
-        <is>
-          <t>[WIL] Studio App Setup</t>
-        </is>
-      </c>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr"/>
       <c r="E79" t="inlineStr">
         <is>
           <t>Done</t>
@@ -3582,13 +3544,7 @@
       </c>
       <c r="F79" t="inlineStr"/>
       <c r="G79" t="inlineStr"/>
-      <c r="H79" t="inlineStr">
-        <is>
-          <t>other: [https://cloud.hypatos.ai/projects/po-extract-agdh8f5s|https://cloud.hypatos.ai/projects/po-extract-agdh8f5s|smart-link] 
-JP [https://cloud.hypatos.ai/projects/po-extract-jp-18lyzmdi|https://cloud.hypatos.ai/projects/po-extract-jp-18lyzmdi|smart-link] 
-valid - see companies</t>
-        </is>
-      </c>
+      <c r="H79" t="inlineStr"/>
       <c r="I79" t="inlineStr"/>
       <c r="J79" t="inlineStr"/>
       <c r="K79" t="inlineStr">
@@ -3600,12 +3556,12 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>SKK-29</t>
+          <t>SKK-26</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>[WIL] endusers to add to studio</t>
+          <t>[WIL] FILL IMP INDEX</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -3633,12 +3589,12 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>SKK-28</t>
+          <t>SKK-25</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Validation Rule - Requirement Sheet - Company Name</t>
+          <t>[WIL] Translation Service - Costs</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -3654,7 +3610,11 @@
       </c>
       <c r="F81" t="inlineStr"/>
       <c r="G81" t="inlineStr"/>
-      <c r="H81" t="inlineStr"/>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t xml:space="preserve">[https://hypatosai.slack.com/archives/C04FX9MN3F1/p1694853778406419?thread_ts=1694760098.313489&amp;cid=C04FX9MN3F1|https://hypatosai.slack.com/archives/C04FX9MN3F1/p1694853778406419?thread_ts=1694760098.313489&amp;cid=C04FX9MN3F1|smart-link] </t>
+        </is>
+      </c>
       <c r="I81" t="inlineStr"/>
       <c r="J81" t="inlineStr"/>
       <c r="K81" t="inlineStr">
@@ -3666,12 +3626,12 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>SKK-27</t>
+          <t>SKK-24</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>[WIL] start imp training</t>
+          <t>[WIL] Duplicate Detection and Routing Rule Documentation in Confluence</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -3687,7 +3647,11 @@
       </c>
       <c r="F82" t="inlineStr"/>
       <c r="G82" t="inlineStr"/>
-      <c r="H82" t="inlineStr"/>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t xml:space="preserve">[https://hypatos.atlassian.net/jira/software/c/projects/COE/boards/137?modal=detail&amp;selectedIssue=COE-604&amp;search=wil|https://hypatos.atlassian.net/jira/software/c/projects/COE/boards/137?modal=detail&amp;selectedIssue=COE-604&amp;search=wil|smart-link] </t>
+        </is>
+      </c>
       <c r="I82" t="inlineStr"/>
       <c r="J82" t="inlineStr"/>
       <c r="K82" t="inlineStr">
@@ -3699,12 +3663,12 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>SKK-26</t>
+          <t>SKK-23</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>[WIL] FILL IMP INDEX</t>
+          <t>[WIL] Duplicate Detection Ticket</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -3720,8 +3684,16 @@
       </c>
       <c r="F83" t="inlineStr"/>
       <c r="G83" t="inlineStr"/>
-      <c r="H83" t="inlineStr"/>
-      <c r="I83" t="inlineStr"/>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t xml:space="preserve">[https://hypatos.atlassian.net/jira/software/c/projects/COE/boards/137?modal=detail&amp;selectedIssue=COE-604&amp;search=wil|https://hypatos.atlassian.net/jira/software/c/projects/COE/boards/137?modal=detail&amp;selectedIssue=COE-604&amp;search=wil|smart-link] </t>
+        </is>
+      </c>
+      <c r="I83" t="inlineStr">
+        <is>
+          <t>stephan.kuche</t>
+        </is>
+      </c>
       <c r="J83" t="inlineStr"/>
       <c r="K83" t="inlineStr">
         <is>
@@ -3732,20 +3704,24 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>SKK-25</t>
+          <t>SKK-22</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>[WIL] Translation Service - Costs</t>
+          <t>add sender country normalization to all gateway projecfts</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Task</t>
-        </is>
-      </c>
-      <c r="D84" t="inlineStr"/>
+          <t>Sub-task</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>[WIL] Studio App Setup</t>
+        </is>
+      </c>
       <c r="E84" t="inlineStr">
         <is>
           <t>Done</t>
@@ -3754,125 +3730,6 @@
       <c r="F84" t="inlineStr"/>
       <c r="G84" t="inlineStr"/>
       <c r="H84" t="inlineStr">
-        <is>
-          <t xml:space="preserve">[https://hypatosai.slack.com/archives/C04FX9MN3F1/p1694853778406419?thread_ts=1694760098.313489&amp;cid=C04FX9MN3F1|https://hypatosai.slack.com/archives/C04FX9MN3F1/p1694853778406419?thread_ts=1694760098.313489&amp;cid=C04FX9MN3F1|smart-link] </t>
-        </is>
-      </c>
-      <c r="I84" t="inlineStr"/>
-      <c r="J84" t="inlineStr"/>
-      <c r="K84" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="inlineStr">
-        <is>
-          <t>SKK-24</t>
-        </is>
-      </c>
-      <c r="B85" t="inlineStr">
-        <is>
-          <t>[WIL] Duplicate Detection and Routing Rule Documentation in Confluence</t>
-        </is>
-      </c>
-      <c r="C85" t="inlineStr">
-        <is>
-          <t>Task</t>
-        </is>
-      </c>
-      <c r="D85" t="inlineStr"/>
-      <c r="E85" t="inlineStr">
-        <is>
-          <t>Done</t>
-        </is>
-      </c>
-      <c r="F85" t="inlineStr"/>
-      <c r="G85" t="inlineStr"/>
-      <c r="H85" t="inlineStr">
-        <is>
-          <t xml:space="preserve">[https://hypatos.atlassian.net/jira/software/c/projects/COE/boards/137?modal=detail&amp;selectedIssue=COE-604&amp;search=wil|https://hypatos.atlassian.net/jira/software/c/projects/COE/boards/137?modal=detail&amp;selectedIssue=COE-604&amp;search=wil|smart-link] </t>
-        </is>
-      </c>
-      <c r="I85" t="inlineStr"/>
-      <c r="J85" t="inlineStr"/>
-      <c r="K85" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="inlineStr">
-        <is>
-          <t>SKK-23</t>
-        </is>
-      </c>
-      <c r="B86" t="inlineStr">
-        <is>
-          <t>[WIL] Duplicate Detection Ticket</t>
-        </is>
-      </c>
-      <c r="C86" t="inlineStr">
-        <is>
-          <t>Task</t>
-        </is>
-      </c>
-      <c r="D86" t="inlineStr"/>
-      <c r="E86" t="inlineStr">
-        <is>
-          <t>Done</t>
-        </is>
-      </c>
-      <c r="F86" t="inlineStr"/>
-      <c r="G86" t="inlineStr"/>
-      <c r="H86" t="inlineStr">
-        <is>
-          <t xml:space="preserve">[https://hypatos.atlassian.net/jira/software/c/projects/COE/boards/137?modal=detail&amp;selectedIssue=COE-604&amp;search=wil|https://hypatos.atlassian.net/jira/software/c/projects/COE/boards/137?modal=detail&amp;selectedIssue=COE-604&amp;search=wil|smart-link] </t>
-        </is>
-      </c>
-      <c r="I86" t="inlineStr">
-        <is>
-          <t>stephan.kuche</t>
-        </is>
-      </c>
-      <c r="J86" t="inlineStr"/>
-      <c r="K86" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="inlineStr">
-        <is>
-          <t>SKK-22</t>
-        </is>
-      </c>
-      <c r="B87" t="inlineStr">
-        <is>
-          <t>add sender country normalization to all gateway projecfts</t>
-        </is>
-      </c>
-      <c r="C87" t="inlineStr">
-        <is>
-          <t>Sub-task</t>
-        </is>
-      </c>
-      <c r="D87" t="inlineStr">
-        <is>
-          <t>[WIL] Studio App Setup</t>
-        </is>
-      </c>
-      <c r="E87" t="inlineStr">
-        <is>
-          <t>Done</t>
-        </is>
-      </c>
-      <c r="F87" t="inlineStr"/>
-      <c r="G87" t="inlineStr"/>
-      <c r="H87" t="inlineStr">
         <is>
           <t>{noformat} "normalization": [
                         {
@@ -3886,76 +3743,76 @@
                     ],{noformat}</t>
         </is>
       </c>
-      <c r="I87" t="inlineStr"/>
-      <c r="J87" t="inlineStr"/>
-      <c r="K87" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="inlineStr">
+      <c r="I84" t="inlineStr"/>
+      <c r="J84" t="inlineStr"/>
+      <c r="K84" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
         <is>
           <t>SKK-21</t>
         </is>
       </c>
-      <c r="B88" t="inlineStr">
+      <c r="B85" t="inlineStr">
         <is>
           <t>[WIL] IMP only for MY, MM, JP</t>
         </is>
       </c>
-      <c r="C88" t="inlineStr">
-        <is>
-          <t>Task</t>
-        </is>
-      </c>
-      <c r="D88" t="inlineStr"/>
-      <c r="E88" t="inlineStr">
-        <is>
-          <t>Done</t>
-        </is>
-      </c>
-      <c r="F88" t="inlineStr"/>
-      <c r="G88" t="inlineStr"/>
-      <c r="H88" t="inlineStr">
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr"/>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr"/>
+      <c r="G85" t="inlineStr"/>
+      <c r="H85" t="inlineStr">
         <is>
           <t xml:space="preserve">Australia and NZ dont need IMP - schema has to be changed </t>
         </is>
       </c>
-      <c r="I88" t="inlineStr"/>
-      <c r="J88" t="inlineStr"/>
-      <c r="K88" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="inlineStr">
+      <c r="I85" t="inlineStr"/>
+      <c r="J85" t="inlineStr"/>
+      <c r="K85" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
         <is>
           <t>SKK-20</t>
         </is>
       </c>
-      <c r="B89" t="inlineStr">
+      <c r="B86" t="inlineStr">
         <is>
           <t>[WIL] MD Filter per project</t>
         </is>
       </c>
-      <c r="C89" t="inlineStr">
-        <is>
-          <t>Task</t>
-        </is>
-      </c>
-      <c r="D89" t="inlineStr"/>
-      <c r="E89" t="inlineStr">
-        <is>
-          <t>Done</t>
-        </is>
-      </c>
-      <c r="F89" t="inlineStr"/>
-      <c r="G89" t="inlineStr"/>
-      <c r="H89" t="inlineStr">
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr"/>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr"/>
+      <c r="G86" t="inlineStr"/>
+      <c r="H86" t="inlineStr">
         <is>
           <t>*Add*
 "options": {
@@ -3963,6 +3820,117 @@
  "companyId": "nameOfYourCompanyCode"</t>
         </is>
       </c>
+      <c r="I86" t="inlineStr"/>
+      <c r="J86" t="inlineStr"/>
+      <c r="K86" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>SKK-19</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>apply validation rules</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Sub-task</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>[WIL] Studio App Setup</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr"/>
+      <c r="G87" t="inlineStr"/>
+      <c r="H87" t="inlineStr"/>
+      <c r="I87" t="inlineStr"/>
+      <c r="J87" t="inlineStr"/>
+      <c r="K87" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>SKK-18</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>reduce datapoints where they are not needed</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Sub-task</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>[WIL] Studio App Setup</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr"/>
+      <c r="G88" t="inlineStr"/>
+      <c r="H88" t="inlineStr"/>
+      <c r="I88" t="inlineStr"/>
+      <c r="J88" t="inlineStr"/>
+      <c r="K88" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>SKK-17</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>apply model to all projects</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Sub-task</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>[WIL] Studio App Setup</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr"/>
+      <c r="G89" t="inlineStr"/>
+      <c r="H89" t="inlineStr"/>
       <c r="I89" t="inlineStr"/>
       <c r="J89" t="inlineStr"/>
       <c r="K89" t="inlineStr">
@@ -3974,24 +3942,20 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>SKK-19</t>
+          <t>SKK-16</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>apply validation rules</t>
+          <t>[WIL] Validation RULES</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Sub-task</t>
-        </is>
-      </c>
-      <c r="D90" t="inlineStr">
-        <is>
-          <t>[WIL] Studio App Setup</t>
-        </is>
-      </c>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr"/>
       <c r="E90" t="inlineStr">
         <is>
           <t>Done</t>
@@ -3999,7 +3963,13 @@
       </c>
       <c r="F90" t="inlineStr"/>
       <c r="G90" t="inlineStr"/>
-      <c r="H90" t="inlineStr"/>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>||*Validation Rule*||*Comment*|| ||
+|Company Name Captured vs Project the invoice was uploaded to|Use Regex to verify if company name is correct| |
+| | | |</t>
+        </is>
+      </c>
       <c r="I90" t="inlineStr"/>
       <c r="J90" t="inlineStr"/>
       <c r="K90" t="inlineStr">
@@ -4011,12 +3981,12 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>SKK-18</t>
+          <t>SKK-15</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>reduce datapoints where they are not needed</t>
+          <t>check after CoE is done</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -4036,120 +4006,7 @@
       </c>
       <c r="F91" t="inlineStr"/>
       <c r="G91" t="inlineStr"/>
-      <c r="H91" t="inlineStr"/>
-      <c r="I91" t="inlineStr"/>
-      <c r="J91" t="inlineStr"/>
-      <c r="K91" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="inlineStr">
-        <is>
-          <t>SKK-17</t>
-        </is>
-      </c>
-      <c r="B92" t="inlineStr">
-        <is>
-          <t>apply model to all projects</t>
-        </is>
-      </c>
-      <c r="C92" t="inlineStr">
-        <is>
-          <t>Sub-task</t>
-        </is>
-      </c>
-      <c r="D92" t="inlineStr">
-        <is>
-          <t>[WIL] Studio App Setup</t>
-        </is>
-      </c>
-      <c r="E92" t="inlineStr">
-        <is>
-          <t>Done</t>
-        </is>
-      </c>
-      <c r="F92" t="inlineStr"/>
-      <c r="G92" t="inlineStr"/>
-      <c r="H92" t="inlineStr"/>
-      <c r="I92" t="inlineStr"/>
-      <c r="J92" t="inlineStr"/>
-      <c r="K92" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="inlineStr">
-        <is>
-          <t>SKK-16</t>
-        </is>
-      </c>
-      <c r="B93" t="inlineStr">
-        <is>
-          <t>[WIL] Validation RULES</t>
-        </is>
-      </c>
-      <c r="C93" t="inlineStr">
-        <is>
-          <t>Task</t>
-        </is>
-      </c>
-      <c r="D93" t="inlineStr"/>
-      <c r="E93" t="inlineStr">
-        <is>
-          <t>Done</t>
-        </is>
-      </c>
-      <c r="F93" t="inlineStr"/>
-      <c r="G93" t="inlineStr"/>
-      <c r="H93" t="inlineStr">
-        <is>
-          <t>||*Validation Rule*||*Comment*|| ||
-|Company Name Captured vs Project the invoice was uploaded to|Use Regex to verify if company name is correct| |
-| | | |</t>
-        </is>
-      </c>
-      <c r="I93" t="inlineStr"/>
-      <c r="J93" t="inlineStr"/>
-      <c r="K93" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="inlineStr">
-        <is>
-          <t>SKK-15</t>
-        </is>
-      </c>
-      <c r="B94" t="inlineStr">
-        <is>
-          <t>check after CoE is done</t>
-        </is>
-      </c>
-      <c r="C94" t="inlineStr">
-        <is>
-          <t>Sub-task</t>
-        </is>
-      </c>
-      <c r="D94" t="inlineStr">
-        <is>
-          <t>[WIL] Studio App Setup</t>
-        </is>
-      </c>
-      <c r="E94" t="inlineStr">
-        <is>
-          <t>Done</t>
-        </is>
-      </c>
-      <c r="F94" t="inlineStr"/>
-      <c r="G94" t="inlineStr"/>
-      <c r="H94" t="inlineStr">
+      <c r="H91" t="inlineStr">
         <is>
           <t xml:space="preserve">* AUS normalization of currency
 * NZ  normalization of currency
@@ -4160,39 +4017,39 @@
 * Derivation according to requirementlist </t>
         </is>
       </c>
-      <c r="I94" t="inlineStr"/>
-      <c r="J94" t="inlineStr"/>
-      <c r="K94" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="inlineStr">
+      <c r="I91" t="inlineStr"/>
+      <c r="J91" t="inlineStr"/>
+      <c r="K91" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
         <is>
           <t>SKK-14</t>
         </is>
       </c>
-      <c r="B95" t="inlineStr">
+      <c r="B92" t="inlineStr">
         <is>
           <t>[KTM] Results Present</t>
         </is>
       </c>
-      <c r="C95" t="inlineStr">
-        <is>
-          <t>Task</t>
-        </is>
-      </c>
-      <c r="D95" t="inlineStr"/>
-      <c r="E95" t="inlineStr">
-        <is>
-          <t>Done</t>
-        </is>
-      </c>
-      <c r="F95" t="inlineStr"/>
-      <c r="G95" t="inlineStr"/>
-      <c r="H95" t="inlineStr">
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr"/>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr"/>
+      <c r="G92" t="inlineStr"/>
+      <c r="H92" t="inlineStr">
         <is>
           <t>0900: documents ids
 64feeea06269a554341ec270 , 64fef939fcd512525a81f15f
@@ -4200,6 +4057,117 @@
 64fef945994edcb6e189166f, 64feeea307197a31d043df31, 64feeeaf488efbf0dff6892f, 64fef934fef6b44fe17c05c1</t>
         </is>
       </c>
+      <c r="I92" t="inlineStr"/>
+      <c r="J92" t="inlineStr"/>
+      <c r="K92" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>SKK-13</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>roll out for all countries</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Sub-task</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>[WIL] Studio App Setup</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr"/>
+      <c r="G93" t="inlineStr"/>
+      <c r="H93" t="inlineStr"/>
+      <c r="I93" t="inlineStr"/>
+      <c r="J93" t="inlineStr"/>
+      <c r="K93" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>SKK-12</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>create routing rules</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Sub-task</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>[WIL] Studio App Setup</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr"/>
+      <c r="G94" t="inlineStr"/>
+      <c r="H94" t="inlineStr"/>
+      <c r="I94" t="inlineStr"/>
+      <c r="J94" t="inlineStr"/>
+      <c r="K94" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>SKK-11</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t xml:space="preserve">add derivation rules </t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>Sub-task</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>[WIL] Studio App Setup</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr"/>
+      <c r="G95" t="inlineStr"/>
+      <c r="H95" t="inlineStr"/>
       <c r="I95" t="inlineStr"/>
       <c r="J95" t="inlineStr"/>
       <c r="K95" t="inlineStr">
@@ -4211,12 +4179,12 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>SKK-13</t>
+          <t>SKK-10</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>roll out for all countries</t>
+          <t>apply normalization</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -4248,12 +4216,12 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>SKK-12</t>
+          <t>SKK-9</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>create routing rules</t>
+          <t>create schemas</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -4285,12 +4253,12 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>SKK-11</t>
+          <t>SKK-8</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t xml:space="preserve">add derivation rules </t>
+          <t>create projects</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -4322,24 +4290,20 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>SKK-10</t>
+          <t>SKK-7</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>apply normalization</t>
+          <t>[WIL] Studio App Setup</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>Sub-task</t>
-        </is>
-      </c>
-      <c r="D99" t="inlineStr">
-        <is>
-          <t>[WIL] Studio App Setup</t>
-        </is>
-      </c>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr"/>
       <c r="E99" t="inlineStr">
         <is>
           <t>Done</t>
@@ -4359,24 +4323,20 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>SKK-9</t>
+          <t>SKK-6</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>create schemas</t>
+          <t>[WIL] Date PostProcessor Normalizations</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>Sub-task</t>
-        </is>
-      </c>
-      <c r="D100" t="inlineStr">
-        <is>
-          <t>[WIL] Studio App Setup</t>
-        </is>
-      </c>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr"/>
       <c r="E100" t="inlineStr">
         <is>
           <t>Done</t>
@@ -4384,110 +4344,7 @@
       </c>
       <c r="F100" t="inlineStr"/>
       <c r="G100" t="inlineStr"/>
-      <c r="H100" t="inlineStr"/>
-      <c r="I100" t="inlineStr"/>
-      <c r="J100" t="inlineStr"/>
-      <c r="K100" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="inlineStr">
-        <is>
-          <t>SKK-8</t>
-        </is>
-      </c>
-      <c r="B101" t="inlineStr">
-        <is>
-          <t>create projects</t>
-        </is>
-      </c>
-      <c r="C101" t="inlineStr">
-        <is>
-          <t>Sub-task</t>
-        </is>
-      </c>
-      <c r="D101" t="inlineStr">
-        <is>
-          <t>[WIL] Studio App Setup</t>
-        </is>
-      </c>
-      <c r="E101" t="inlineStr">
-        <is>
-          <t>Done</t>
-        </is>
-      </c>
-      <c r="F101" t="inlineStr"/>
-      <c r="G101" t="inlineStr"/>
-      <c r="H101" t="inlineStr"/>
-      <c r="I101" t="inlineStr"/>
-      <c r="J101" t="inlineStr"/>
-      <c r="K101" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" t="inlineStr">
-        <is>
-          <t>SKK-7</t>
-        </is>
-      </c>
-      <c r="B102" t="inlineStr">
-        <is>
-          <t>[WIL] Studio App Setup</t>
-        </is>
-      </c>
-      <c r="C102" t="inlineStr">
-        <is>
-          <t>Task</t>
-        </is>
-      </c>
-      <c r="D102" t="inlineStr"/>
-      <c r="E102" t="inlineStr">
-        <is>
-          <t>Done</t>
-        </is>
-      </c>
-      <c r="F102" t="inlineStr"/>
-      <c r="G102" t="inlineStr"/>
-      <c r="H102" t="inlineStr"/>
-      <c r="I102" t="inlineStr"/>
-      <c r="J102" t="inlineStr"/>
-      <c r="K102" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" t="inlineStr">
-        <is>
-          <t>SKK-6</t>
-        </is>
-      </c>
-      <c r="B103" t="inlineStr">
-        <is>
-          <t>[WIL] Date PostProcessor Normalizations</t>
-        </is>
-      </c>
-      <c r="C103" t="inlineStr">
-        <is>
-          <t>Task</t>
-        </is>
-      </c>
-      <c r="D103" t="inlineStr"/>
-      <c r="E103" t="inlineStr">
-        <is>
-          <t>Done</t>
-        </is>
-      </c>
-      <c r="F103" t="inlineStr"/>
-      <c r="G103" t="inlineStr"/>
-      <c r="H103" t="inlineStr">
+      <c r="H100" t="inlineStr">
         <is>
           <t>||*Country*||*URL*||*Issued AT*||
 |JP|[https://cloud.hypatos.ai/projects/jp-annotation-samples-i6jvtmw1/64f1bc448eb05f6d04c9ffc6|https://cloud.hypatos.ai/projects/jp-annotation-samples-i6jvtmw1/64f1bc448eb05f6d04c9ffc6|smart-link]|2023 年 4 月 3 日|
@@ -4504,72 +4361,72 @@
 | | | |</t>
         </is>
       </c>
-      <c r="I103" t="inlineStr"/>
-      <c r="J103" t="inlineStr"/>
-      <c r="K103" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" t="inlineStr">
+      <c r="I100" t="inlineStr"/>
+      <c r="J100" t="inlineStr"/>
+      <c r="K100" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
         <is>
           <t>SKK-5</t>
         </is>
       </c>
-      <c r="B104" t="inlineStr">
+      <c r="B101" t="inlineStr">
         <is>
           <t>[WIL] IMP</t>
         </is>
       </c>
-      <c r="C104" t="inlineStr">
-        <is>
-          <t>Task</t>
-        </is>
-      </c>
-      <c r="D104" t="inlineStr"/>
-      <c r="E104" t="inlineStr">
-        <is>
-          <t>Done</t>
-        </is>
-      </c>
-      <c r="F104" t="inlineStr"/>
-      <c r="G104" t="inlineStr"/>
-      <c r="H104" t="inlineStr"/>
-      <c r="I104" t="inlineStr"/>
-      <c r="J104" t="inlineStr"/>
-      <c r="K104" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" t="inlineStr">
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr"/>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="F101" t="inlineStr"/>
+      <c r="G101" t="inlineStr"/>
+      <c r="H101" t="inlineStr"/>
+      <c r="I101" t="inlineStr"/>
+      <c r="J101" t="inlineStr"/>
+      <c r="K101" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
         <is>
           <t>SKK-4</t>
         </is>
       </c>
-      <c r="B105" t="inlineStr">
+      <c r="B102" t="inlineStr">
         <is>
           <t>[PlayGround] Transformer</t>
         </is>
       </c>
-      <c r="C105" t="inlineStr">
-        <is>
-          <t>Task</t>
-        </is>
-      </c>
-      <c r="D105" t="inlineStr"/>
-      <c r="E105" t="inlineStr">
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr"/>
+      <c r="E102" t="inlineStr">
         <is>
           <t>Blocked</t>
         </is>
       </c>
-      <c r="F105" t="inlineStr"/>
-      <c r="G105" t="inlineStr"/>
-      <c r="H105" t="inlineStr">
+      <c r="F102" t="inlineStr"/>
+      <c r="G102" t="inlineStr"/>
+      <c r="H102" t="inlineStr">
         <is>
           <t xml:space="preserve">cl-deployment-gpt-demo-production
 cl-deployment-gpt-demo-3-5-production
@@ -4583,39 +4440,39 @@
 ** Everytime we call OpenAI API - we iterate over a confirmed document to send the context </t>
         </is>
       </c>
-      <c r="I105" t="inlineStr"/>
-      <c r="J105" t="inlineStr"/>
-      <c r="K105" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" t="inlineStr">
+      <c r="I102" t="inlineStr"/>
+      <c r="J102" t="inlineStr"/>
+      <c r="K102" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
         <is>
           <t>SKK-3</t>
         </is>
       </c>
-      <c r="B106" t="inlineStr">
+      <c r="B103" t="inlineStr">
         <is>
           <t>[OKR] Meeting with Hé</t>
         </is>
       </c>
-      <c r="C106" t="inlineStr">
-        <is>
-          <t>Task</t>
-        </is>
-      </c>
-      <c r="D106" t="inlineStr"/>
-      <c r="E106" t="inlineStr">
-        <is>
-          <t>Done</t>
-        </is>
-      </c>
-      <c r="F106" t="inlineStr"/>
-      <c r="G106" t="inlineStr"/>
-      <c r="H106" t="inlineStr">
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr"/>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="F103" t="inlineStr"/>
+      <c r="G103" t="inlineStr"/>
+      <c r="H103" t="inlineStr">
         <is>
           <t xml:space="preserve">*KR*
 * _Design a company-wide transition plan to migrate all accounts to google OCR within three months_
@@ -4665,72 +4522,72 @@
 *  </t>
         </is>
       </c>
-      <c r="I106" t="inlineStr"/>
-      <c r="J106" t="inlineStr"/>
-      <c r="K106" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" t="inlineStr">
+      <c r="I103" t="inlineStr"/>
+      <c r="J103" t="inlineStr"/>
+      <c r="K103" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
         <is>
           <t>SKK-2</t>
         </is>
       </c>
-      <c r="B107" t="inlineStr">
+      <c r="B104" t="inlineStr">
         <is>
           <t>[WIL] Routing</t>
         </is>
       </c>
-      <c r="C107" t="inlineStr">
-        <is>
-          <t>Task</t>
-        </is>
-      </c>
-      <c r="D107" t="inlineStr"/>
-      <c r="E107" t="inlineStr">
-        <is>
-          <t>Done</t>
-        </is>
-      </c>
-      <c r="F107" t="inlineStr"/>
-      <c r="G107" t="inlineStr"/>
-      <c r="H107" t="inlineStr"/>
-      <c r="I107" t="inlineStr"/>
-      <c r="J107" t="inlineStr"/>
-      <c r="K107" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" t="inlineStr">
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr"/>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="F104" t="inlineStr"/>
+      <c r="G104" t="inlineStr"/>
+      <c r="H104" t="inlineStr"/>
+      <c r="I104" t="inlineStr"/>
+      <c r="J104" t="inlineStr"/>
+      <c r="K104" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
         <is>
           <t>SKK-1</t>
         </is>
       </c>
-      <c r="B108" t="inlineStr">
+      <c r="B105" t="inlineStr">
         <is>
           <t>[WIL] Normalizations JPY</t>
         </is>
       </c>
-      <c r="C108" t="inlineStr">
-        <is>
-          <t>Task</t>
-        </is>
-      </c>
-      <c r="D108" t="inlineStr"/>
-      <c r="E108" t="inlineStr">
-        <is>
-          <t>Done</t>
-        </is>
-      </c>
-      <c r="F108" t="inlineStr"/>
-      <c r="G108" t="inlineStr"/>
-      <c r="H108" t="inlineStr">
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>Task</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr"/>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr"/>
+      <c r="G105" t="inlineStr"/>
+      <c r="H105" t="inlineStr">
         <is>
           <t>||*Country*||*Datapoint*||*URL*||*Comment*||*Exp. Result*||*Done*||
 |JP|Currency|[https://cloud.hypatos.ai/projects/jp-annotation-samples-i6jvtmw1/64f183153236d7d78e7ca75f|https://cloud.hypatos.ai/projects/jp-annotation-samples-i6jvtmw1/64f183153236d7d78e7ca75f|smart-link]|{{[^a-zA-Z]+([Jj]py|JPY)+|([Jj]py|JPY)+[^a-zA-Z]+|¥|^([Jj]py|JPY)+$}}|JPY|x|
@@ -4742,9 +4599,9 @@
 is this invoice? - no| |y|</t>
         </is>
       </c>
-      <c r="I108" t="inlineStr"/>
-      <c r="J108" t="inlineStr"/>
-      <c r="K108" t="inlineStr">
+      <c r="I105" t="inlineStr"/>
+      <c r="J105" t="inlineStr"/>
+      <c r="K105" t="inlineStr">
         <is>
           <t>[]</t>
         </is>

</xml_diff>

<commit_message>
added functionality to provide a project name when creating a project
</commit_message>
<xml_diff>
--- a/templates/jiraissues.xlsx
+++ b/templates/jiraissues.xlsx
@@ -493,7 +493,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>TD-7102</t>
+          <t>TD-7208</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -542,7 +542,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>TD-7101</t>
+          <t>TD-7207</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -591,7 +591,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>TD-7100</t>
+          <t>TD-7206</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -640,7 +640,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>TD-7099</t>
+          <t>TD-7205</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -689,7 +689,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>TD-7098</t>
+          <t>TD-7204</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -738,7 +738,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>TD-7097</t>
+          <t>TD-7203</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -753,7 +753,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Pilot</t>
+          <t>PILOTWIL</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -787,7 +787,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>TD-7096</t>
+          <t>TD-7202</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -836,7 +836,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>TD-7095</t>
+          <t>TD-7201</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -885,7 +885,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>TD-7094</t>
+          <t>TD-7200</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -934,7 +934,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>TD-7093</t>
+          <t>TD-7199</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -983,7 +983,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>TD-7092</t>
+          <t>TD-7198</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1032,7 +1032,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>TD-7091</t>
+          <t>TD-7197</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1047,7 +1047,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Pilot</t>
+          <t>PILOTWIL</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -1081,7 +1081,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>TD-7090</t>
+          <t>TD-7196</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1130,7 +1130,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>TD-7089</t>
+          <t>TD-7195</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1179,7 +1179,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>TD-7088</t>
+          <t>TD-7194</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1228,7 +1228,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>TD-7087</t>
+          <t>TD-7193</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1243,7 +1243,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Pilot</t>
+          <t>PILOTWIL</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1277,7 +1277,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>TD-7086</t>
+          <t>TD-7192</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1326,7 +1326,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>TD-7085</t>
+          <t>TD-7191</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1375,7 +1375,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>TD-7084</t>
+          <t>TD-7190</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1424,7 +1424,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>TD-7083</t>
+          <t>TD-7189</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1473,7 +1473,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>TD-7082</t>
+          <t>TD-7188</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1522,7 +1522,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>TD-7081</t>
+          <t>TD-7187</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1537,7 +1537,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Pilot</t>
+          <t>PILOTWIL</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1571,7 +1571,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>TD-7080</t>
+          <t>TD-7186</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1620,7 +1620,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>TD-7079</t>
+          <t>TD-7185</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1669,7 +1669,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>TD-7078</t>
+          <t>TD-7184</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1684,7 +1684,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Pilot</t>
+          <t>PILOTWIL</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1718,7 +1718,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>TD-7077</t>
+          <t>TD-7183</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1767,7 +1767,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>TD-7076</t>
+          <t>TD-7182</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1816,7 +1816,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>TD-7075</t>
+          <t>TD-7181</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1831,7 +1831,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Pilot</t>
+          <t>PILOTWIL</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -1865,7 +1865,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>TD-7074</t>
+          <t>TD-7180</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1914,7 +1914,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>TD-7073</t>
+          <t>TD-7179</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1963,7 +1963,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>TD-7072</t>
+          <t>TD-7178</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -2012,7 +2012,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>TD-7071</t>
+          <t>TD-7177</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -2027,7 +2027,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Pilot</t>
+          <t>PILOTWIL</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -2061,7 +2061,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>TD-7070</t>
+          <t>TD-7176</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -2110,7 +2110,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>TD-7069</t>
+          <t>TD-7175</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -2159,7 +2159,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>TD-7068</t>
+          <t>TD-7174</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -2174,7 +2174,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Pilot</t>
+          <t>PILOTWIL</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -2208,7 +2208,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>TD-7067</t>
+          <t>TD-7173</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -2257,7 +2257,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>TD-7066</t>
+          <t>TD-7172</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -2272,7 +2272,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Pilot</t>
+          <t>PILOTWIL</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -2306,12 +2306,12 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>TD-7065</t>
+          <t>TD-7171</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Pilot</t>
+          <t>PILOTWIL</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">

</xml_diff>